<commit_message>
App working as expected
</commit_message>
<xml_diff>
--- a/Details.xlsx
+++ b/Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vibhas\Desktop\Vibhas\Courses\MassEmailer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F258BE-7D28-455A-852E-5976E1AF9214}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFBA413-93AC-42BC-9F8C-15B2EBD47397}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,27 +25,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>S.No.</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>john@doe.com</t>
-  </si>
-  <si>
-    <t>Mike Tyrell</t>
-  </si>
-  <si>
-    <t>mike@tyrell.com</t>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Tyrell</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Amount Due</t>
+  </si>
+  <si>
+    <t>x@gmail.com</t>
+  </si>
+  <si>
+    <t>y@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -390,57 +402,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.21875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="3" width="21.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="43.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{FD077FBD-79F7-4887-8500-7F836821434D}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{9BE4006F-F862-4D6D-A0E3-AEF3BA8DE916}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{FD077FBD-79F7-4887-8500-7F836821434D}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{9BE4006F-F862-4D6D-A0E3-AEF3BA8DE916}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactored code to open and close connection only once
</commit_message>
<xml_diff>
--- a/Details.xlsx
+++ b/Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vibhas\Desktop\Vibhas\Courses\MassEmailer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFBA413-93AC-42BC-9F8C-15B2EBD47397}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7928EA-9392-42D1-979F-5DF11062CB7B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>S.No.</t>
   </si>
@@ -52,19 +52,13 @@
   </si>
   <si>
     <t>Amount Due</t>
-  </si>
-  <si>
-    <t>x@gmail.com</t>
-  </si>
-  <si>
-    <t>y@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,14 +70,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,9 +92,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -118,12 +103,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -405,7 +389,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,9 +428,7 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="1">
         <v>30</v>
       </c>
@@ -461,18 +443,12 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="1">
         <v>60</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{FD077FBD-79F7-4887-8500-7F836821434D}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{9BE4006F-F862-4D6D-A0E3-AEF3BA8DE916}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>